<commit_message>
Update result2.xlsx with new optimization results
- Modified the Excel file to reflect the latest optimization outcomes from the genetic algorithm and PSO scripts.
- This update ensures that the results are consistent with recent changes in the optimization logic and parameters.
</commit_message>
<xml_diff>
--- a/附件/result2.xlsx
+++ b/附件/result2.xlsx
@@ -1,124 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\2024-5-1\数学建模竞赛组委会、专家组工作\竞赛2025\A题-烟幕干扰弹投放策略\2025-8-23-3 A题(蔡志杰)\附件\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DDF92F2-BB74-42CA-B380-B52D47D03171}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
-      <xlwcv:version setVersion="1"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
-  <si>
-    <t>无人机编号</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>无人机运动方向</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>无人机运动速度 (m/s)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>烟幕干扰弹投放点的x坐标 (m)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>烟幕干扰弹投放点的y坐标 (m)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>烟幕干扰弹投放点的z坐标 (m)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>烟幕干扰弹起爆点的x坐标 (m)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>烟幕干扰弹起爆点的y坐标 (m)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>烟幕干扰弹起爆点的z坐标 (m)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>有效干扰时长 (s)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>注：以x轴为正向，逆时针方向为正，取值0~360（度）。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FY1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FY2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FY3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
+      <name val="等线"/>
+      <charset val="134"/>
+      <family val="2"/>
+      <color theme="1"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <family val="2"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="等线"/>
+      <charset val="134"/>
+      <family val="2"/>
       <sz val="9"/>
-      <name val="等线"/>
-      <family val="2"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -134,37 +51,97 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -484,78 +461,232 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="13.58203125" customWidth="1"/>
-    <col min="2" max="2" width="17.58203125" customWidth="1"/>
-    <col min="3" max="3" width="16.58203125" customWidth="1"/>
-    <col min="4" max="10" width="14.58203125" customWidth="1"/>
+    <col width="13.58203125" customWidth="1" style="4" min="1" max="1"/>
+    <col width="17.58203125" customWidth="1" style="4" min="2" max="2"/>
+    <col width="16.58203125" customWidth="1" style="4" min="3" max="3"/>
+    <col width="14.58203125" customWidth="1" style="4" min="4" max="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="28" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
-    </row>
-    <row r="6" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
-      <c r="B6" s="2" t="s">
-        <v>10</v>
+    <row r="1" ht="28" customFormat="1" customHeight="1" s="2">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>无人机编号</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>无人机运动方向</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>无人机运动速度 (m/s)</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>烟幕干扰弹投放点的x坐标 (m)</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>烟幕干扰弹投放点的y坐标 (m)</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>烟幕干扰弹投放点的z坐标 (m)</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>烟幕干扰弹起爆点的x坐标 (m)</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>烟幕干扰弹起爆点的y坐标 (m)</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>烟幕干扰弹起爆点的z坐标 (m)</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>有效干扰时长 (s)</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="inlineStr">
+        <is>
+          <t>FY1</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t>FY2</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="inlineStr">
+        <is>
+          <t>FY3</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="n"/>
+    </row>
+    <row r="6" ht="60" customHeight="1" s="4">
+      <c r="A6" s="1" t="n"/>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>注：以x轴为正向，逆时针方向为正，取值0~360（度）。</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>FY1</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>5.26</v>
+      </c>
+      <c r="C7" t="n">
+        <v>140</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.881</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="F7" t="n">
+        <v>17922.792</v>
+      </c>
+      <c r="G7" t="n">
+        <v>11.304</v>
+      </c>
+      <c r="H7" t="n">
+        <v>1800</v>
+      </c>
+      <c r="I7" t="n">
+        <v>17923.489</v>
+      </c>
+      <c r="J7" t="n">
+        <v>11.368</v>
+      </c>
+      <c r="K7" t="n">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>FY2</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>204.427</v>
+      </c>
+      <c r="C8" t="n">
+        <v>138.431</v>
+      </c>
+      <c r="D8" t="n">
+        <v>13.625</v>
+      </c>
+      <c r="E8" t="n">
+        <v>9.965</v>
+      </c>
+      <c r="F8" t="n">
+        <v>10282.708</v>
+      </c>
+      <c r="G8" t="n">
+        <v>620.013</v>
+      </c>
+      <c r="H8" t="n">
+        <v>1400</v>
+      </c>
+      <c r="I8" t="n">
+        <v>9026.785</v>
+      </c>
+      <c r="J8" t="n">
+        <v>49.579</v>
+      </c>
+      <c r="K8" t="n">
+        <v>913.139</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>FY3</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>189.496</v>
+      </c>
+      <c r="C9" t="n">
+        <v>90.919</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.334</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="F9" t="n">
+        <v>5970.06</v>
+      </c>
+      <c r="G9" t="n">
+        <v>-3005.008</v>
+      </c>
+      <c r="H9" t="n">
+        <v>700</v>
+      </c>
+      <c r="I9" t="n">
+        <v>5969.612</v>
+      </c>
+      <c r="J9" t="n">
+        <v>-3005.083</v>
+      </c>
+      <c r="K9" t="n">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>总有效遮蔽并集时长(s)</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>9.057</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Remove obsolete files and update requirements
- Deleted GEMINI.md, problem.md, and several Python scripts related to smoke bomb optimization to streamline the project structure.
- Updated requirements.txt to remove openpyxl, reflecting the current dependencies needed for the project.
- This cleanup is part of ongoing efforts to enhance code maintainability and focus on essential components.
</commit_message>
<xml_diff>
--- a/附件/result2.xlsx
+++ b/附件/result2.xlsx
@@ -466,7 +466,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -565,124 +565,487 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" s="0" t="inlineStr">
         <is>
           <t>FY1</t>
         </is>
       </c>
-      <c r="B7" t="n">
+      <c r="B7" s="0" t="n">
         <v>5.26</v>
       </c>
-      <c r="C7" t="n">
+      <c r="C7" s="0" t="n">
         <v>140</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D7" s="0" t="n">
         <v>0.881</v>
       </c>
-      <c r="E7" t="n">
+      <c r="E7" s="0" t="n">
         <v>0.005</v>
       </c>
-      <c r="F7" t="n">
+      <c r="F7" s="0" t="n">
         <v>17922.792</v>
       </c>
-      <c r="G7" t="n">
+      <c r="G7" s="0" t="n">
         <v>11.304</v>
       </c>
-      <c r="H7" t="n">
+      <c r="H7" s="0" t="n">
         <v>1800</v>
       </c>
-      <c r="I7" t="n">
+      <c r="I7" s="0" t="n">
         <v>17923.489</v>
       </c>
-      <c r="J7" t="n">
+      <c r="J7" s="0" t="n">
         <v>11.368</v>
       </c>
-      <c r="K7" t="n">
+      <c r="K7" s="0" t="n">
         <v>1800</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A8" s="0" t="inlineStr">
         <is>
           <t>FY2</t>
         </is>
       </c>
-      <c r="B8" t="n">
+      <c r="B8" s="0" t="n">
         <v>204.427</v>
       </c>
-      <c r="C8" t="n">
+      <c r="C8" s="0" t="n">
         <v>138.431</v>
       </c>
-      <c r="D8" t="n">
+      <c r="D8" s="0" t="n">
         <v>13.625</v>
       </c>
-      <c r="E8" t="n">
+      <c r="E8" s="0" t="n">
         <v>9.965</v>
       </c>
-      <c r="F8" t="n">
+      <c r="F8" s="0" t="n">
         <v>10282.708</v>
       </c>
-      <c r="G8" t="n">
+      <c r="G8" s="0" t="n">
         <v>620.013</v>
       </c>
-      <c r="H8" t="n">
+      <c r="H8" s="0" t="n">
         <v>1400</v>
       </c>
-      <c r="I8" t="n">
+      <c r="I8" s="0" t="n">
         <v>9026.785</v>
       </c>
-      <c r="J8" t="n">
+      <c r="J8" s="0" t="n">
         <v>49.579</v>
       </c>
-      <c r="K8" t="n">
+      <c r="K8" s="0" t="n">
         <v>913.139</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9" s="0" t="inlineStr">
         <is>
           <t>FY3</t>
         </is>
       </c>
-      <c r="B9" t="n">
+      <c r="B9" s="0" t="n">
         <v>189.496</v>
       </c>
-      <c r="C9" t="n">
+      <c r="C9" s="0" t="n">
         <v>90.919</v>
       </c>
-      <c r="D9" t="n">
+      <c r="D9" s="0" t="n">
         <v>0.334</v>
       </c>
-      <c r="E9" t="n">
+      <c r="E9" s="0" t="n">
         <v>0.005</v>
       </c>
-      <c r="F9" t="n">
+      <c r="F9" s="0" t="n">
         <v>5970.06</v>
       </c>
-      <c r="G9" t="n">
+      <c r="G9" s="0" t="n">
         <v>-3005.008</v>
       </c>
-      <c r="H9" t="n">
+      <c r="H9" s="0" t="n">
         <v>700</v>
       </c>
-      <c r="I9" t="n">
+      <c r="I9" s="0" t="n">
         <v>5969.612</v>
       </c>
-      <c r="J9" t="n">
+      <c r="J9" s="0" t="n">
         <v>-3005.083</v>
       </c>
-      <c r="K9" t="n">
+      <c r="K9" s="0" t="n">
         <v>700</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="A10" s="0" t="inlineStr">
         <is>
           <t>总有效遮蔽并集时长(s)</t>
         </is>
       </c>
-      <c r="B10" t="n">
+      <c r="B10" s="0" t="n">
         <v>9.057</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="inlineStr">
+        <is>
+          <t>FY1</t>
+        </is>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>5.3</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>140</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>0.879</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>17922.58</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>11.372</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <v>1800</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>17923.277</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <v>11.437</v>
+      </c>
+      <c r="K11" s="0" t="n">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="inlineStr">
+        <is>
+          <t>FY2</t>
+        </is>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>204.45</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>138.335</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>13.554</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>9.970000000000001</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>10293.109</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>623.92</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>1400</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>9037.578</v>
+      </c>
+      <c r="J12" s="0" t="n">
+        <v>53.062</v>
+      </c>
+      <c r="K12" s="0" t="n">
+        <v>912.592</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="inlineStr">
+        <is>
+          <t>FY3</t>
+        </is>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>199.812</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>90.834</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>5971.546</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <v>-3010.251</v>
+      </c>
+      <c r="H13" s="0" t="n">
+        <v>700</v>
+      </c>
+      <c r="I13" s="0" t="n">
+        <v>5971.119</v>
+      </c>
+      <c r="J13" s="0" t="n">
+        <v>-3010.405</v>
+      </c>
+      <c r="K13" s="0" t="n">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="inlineStr">
+        <is>
+          <t>总有效遮蔽并集时长(s)</t>
+        </is>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>9.138</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="inlineStr">
+        <is>
+          <t>FY1</t>
+        </is>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>5.3</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>140</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>0.879</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>17922.58</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <v>11.372</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <v>1800</v>
+      </c>
+      <c r="I15" s="0" t="n">
+        <v>17923.277</v>
+      </c>
+      <c r="J15" s="0" t="n">
+        <v>11.437</v>
+      </c>
+      <c r="K15" s="0" t="n">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="inlineStr">
+        <is>
+          <t>FY2</t>
+        </is>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>204.45</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>138.335</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>13.554</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>9.970000000000001</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>10293.109</v>
+      </c>
+      <c r="G16" s="0" t="n">
+        <v>623.92</v>
+      </c>
+      <c r="H16" s="0" t="n">
+        <v>1400</v>
+      </c>
+      <c r="I16" s="0" t="n">
+        <v>9037.578</v>
+      </c>
+      <c r="J16" s="0" t="n">
+        <v>53.062</v>
+      </c>
+      <c r="K16" s="0" t="n">
+        <v>912.592</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="inlineStr">
+        <is>
+          <t>FY3</t>
+        </is>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>199.812</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>90.834</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>5971.546</v>
+      </c>
+      <c r="G17" s="0" t="n">
+        <v>-3010.251</v>
+      </c>
+      <c r="H17" s="0" t="n">
+        <v>700</v>
+      </c>
+      <c r="I17" s="0" t="n">
+        <v>5971.119</v>
+      </c>
+      <c r="J17" s="0" t="n">
+        <v>-3010.405</v>
+      </c>
+      <c r="K17" s="0" t="n">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="inlineStr">
+        <is>
+          <t>总有效遮蔽并集时长(s)</t>
+        </is>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>9.138</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>FY1</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>5.326</v>
+      </c>
+      <c r="C19" t="n">
+        <v>140</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.881</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="F19" t="n">
+        <v>17922.874</v>
+      </c>
+      <c r="G19" t="n">
+        <v>11.454</v>
+      </c>
+      <c r="H19" t="n">
+        <v>1800</v>
+      </c>
+      <c r="I19" t="n">
+        <v>17923.571</v>
+      </c>
+      <c r="J19" t="n">
+        <v>11.519</v>
+      </c>
+      <c r="K19" t="n">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>FY2</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>204.53</v>
+      </c>
+      <c r="C20" t="n">
+        <v>138.572</v>
+      </c>
+      <c r="D20" t="n">
+        <v>13.499</v>
+      </c>
+      <c r="E20" t="n">
+        <v>9.951000000000001</v>
+      </c>
+      <c r="F20" t="n">
+        <v>10298.25</v>
+      </c>
+      <c r="G20" t="n">
+        <v>623.409</v>
+      </c>
+      <c r="H20" t="n">
+        <v>1400</v>
+      </c>
+      <c r="I20" t="n">
+        <v>9043.773999999999</v>
+      </c>
+      <c r="J20" t="n">
+        <v>50.93</v>
+      </c>
+      <c r="K20" t="n">
+        <v>914.462</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>FY3</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>175.174</v>
+      </c>
+      <c r="C21" t="n">
+        <v>91.06699999999999</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.347</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="F21" t="n">
+        <v>5968.532</v>
+      </c>
+      <c r="G21" t="n">
+        <v>-2997.343</v>
+      </c>
+      <c r="H21" t="n">
+        <v>700</v>
+      </c>
+      <c r="I21" t="n">
+        <v>5968.078</v>
+      </c>
+      <c r="J21" t="n">
+        <v>-2997.305</v>
+      </c>
+      <c r="K21" t="n">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>总有效遮蔽并集时长(s)</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>9.068</v>
       </c>
     </row>
   </sheetData>

</xml_diff>